<commit_message>
(1) 新增stacked chart 及相關函式的docstring。
Signed-off-by: Joseph <036303@dragonsteel.com.tw>
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tag reference" sheetId="9" r:id="rId1"/>
@@ -8523,7 +8523,7 @@
   <sheetPr codeName="工作表7"/>
   <dimension ref="A1:G236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C210" sqref="C210"/>
     </sheetView>
   </sheetViews>
@@ -12269,10 +12269,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -12424,22 +12424,85 @@
       <c r="E19" s="95"/>
     </row>
     <row r="20" spans="1:5">
+      <c r="A20" s="3">
+        <v>45778</v>
+      </c>
       <c r="E20" s="95"/>
     </row>
     <row r="21" spans="1:5">
+      <c r="A21" s="3">
+        <v>45936</v>
+      </c>
       <c r="E21" s="95"/>
     </row>
     <row r="22" spans="1:5">
+      <c r="A22" s="3">
+        <v>45940</v>
+      </c>
       <c r="E22" s="95"/>
     </row>
     <row r="23" spans="1:5">
+      <c r="A23" s="3">
+        <v>46016</v>
+      </c>
       <c r="E23" s="95"/>
     </row>
     <row r="24" spans="1:5">
+      <c r="A24" s="3">
+        <v>46023</v>
+      </c>
       <c r="E24" s="95"/>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25" s="3">
+        <v>46069</v>
+      </c>
       <c r="E25" s="95"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3">
+        <v>46070</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3">
+        <v>46071</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3">
+        <v>46072</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3">
+        <v>46073</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3">
+        <v>46143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3">
+        <v>46192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3">
+        <v>46290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3">
+        <v>46293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3">
+        <v>46381</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>